<commit_message>
category dealer, category showroom, category listing
</commit_message>
<xml_diff>
--- a/Business Category List.xlsx
+++ b/Business Category List.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\html-template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\html-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44D4120-2748-4028-8A7B-593E7094DD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
   <si>
     <t>Event Organizer</t>
   </si>
@@ -241,12 +240,21 @@
   </si>
   <si>
     <t>Farhan</t>
+  </si>
+  <si>
+    <t>showroom</t>
+  </si>
+  <si>
+    <t>dealer</t>
+  </si>
+  <si>
+    <t>listing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -592,11 +600,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,6 +788,15 @@
       <c r="B12" t="s">
         <v>7</v>
       </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -788,6 +805,15 @@
       <c r="B13" t="s">
         <v>8</v>
       </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -795,6 +821,15 @@
       </c>
       <c r="B14" t="s">
         <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add template Building Bussines Engineering Finance
</commit_message>
<xml_diff>
--- a/Business Category List.xlsx
+++ b/Business Category List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\html-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B66AEFE-FF48-4B7A-82A1-4DDC66302BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -254,7 +255,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -600,10 +601,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="94" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
menambahkan 6 category baru
</commit_message>
<xml_diff>
--- a/Business Category List.xlsx
+++ b/Business Category List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\html-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B66AEFE-FF48-4B7A-82A1-4DDC66302BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47F090D-1FF9-4753-89ED-417C8C867012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
   <si>
     <t>Event Organizer</t>
   </si>
@@ -250,6 +250,75 @@
   </si>
   <si>
     <t>listing</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>machinery</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>renovation</t>
+  </si>
+  <si>
+    <t>contractor</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>manufacturing</t>
+  </si>
+  <si>
+    <t>building</t>
+  </si>
+  <si>
+    <t>factory</t>
+  </si>
+  <si>
+    <t>engineering</t>
+  </si>
+  <si>
+    <t>business</t>
+  </si>
+  <si>
+    <t>construction</t>
+  </si>
+  <si>
+    <t>finance</t>
+  </si>
+  <si>
+    <t>landing page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krisna </t>
+  </si>
+  <si>
+    <t>real estate</t>
+  </si>
+  <si>
+    <t>agency</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>consulting</t>
+  </si>
+  <si>
+    <t>startup</t>
+  </si>
+  <si>
+    <t>ecommerce</t>
+  </si>
+  <si>
+    <t>industrial</t>
   </si>
 </sst>
 </file>
@@ -604,28 +673,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="94" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -645,7 +714,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -665,7 +734,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -685,7 +754,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -705,7 +774,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -725,7 +794,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -745,7 +814,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -765,7 +834,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -782,7 +851,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -799,7 +868,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -816,7 +885,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -833,7 +902,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -841,7 +910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -858,7 +927,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -866,7 +935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -874,7 +943,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -882,7 +951,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -890,7 +959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -898,7 +967,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -906,15 +975,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -931,55 +1009,103 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
@@ -996,124 +1122,169 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
       <c r="B32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
       <c r="B33" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>30</v>
       </c>
       <c r="B34" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
       <c r="B35" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>32</v>
       </c>
       <c r="B36" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>33</v>
       </c>
       <c r="B37" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>34</v>
       </c>
       <c r="B38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>35</v>
       </c>
       <c r="B39" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>37</v>
       </c>
       <c r="B41" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>38</v>
       </c>
       <c r="B42" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>39</v>
       </c>
       <c r="B43" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>40</v>
       </c>
       <c r="B44" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>41</v>
       </c>
       <c r="B45" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>42</v>
       </c>
       <c r="B46" t="s">
         <v>41</v>
+      </c>
+      <c r="C46" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add projek yang kurang
</commit_message>
<xml_diff>
--- a/Business Category List.xlsx
+++ b/Business Category List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\html-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B592620-9598-4DF4-A097-58140556E14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2C439D-0717-4548-A182-F81726A22974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="99">
   <si>
     <t>Event Organizer</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>industrial</t>
+  </si>
+  <si>
+    <t>Fahri</t>
   </si>
 </sst>
 </file>
@@ -673,28 +676,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="94" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="94" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="2" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -714,7 +717,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -734,7 +737,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -754,7 +757,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -774,7 +777,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -794,7 +797,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -814,7 +817,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -834,7 +837,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -851,7 +854,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -868,7 +871,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>
@@ -885,7 +888,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10</v>
       </c>
@@ -902,7 +905,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
@@ -910,7 +913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>12</v>
       </c>
@@ -927,7 +930,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
@@ -935,7 +938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
@@ -943,7 +946,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15</v>
       </c>
@@ -951,7 +954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>16</v>
       </c>
@@ -959,7 +962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17</v>
       </c>
@@ -967,7 +970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>18</v>
       </c>
@@ -975,7 +978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>19</v>
       </c>
@@ -992,7 +995,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1026,7 +1029,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1043,7 +1046,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>23</v>
       </c>
@@ -1060,7 +1063,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>24</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>27</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>28</v>
       </c>
@@ -1138,8 +1141,14 @@
       <c r="C32" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>29</v>
       </c>
@@ -1149,8 +1158,14 @@
       <c r="C33" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>30</v>
       </c>
@@ -1160,8 +1175,14 @@
       <c r="C34" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>31</v>
       </c>
@@ -1171,8 +1192,14 @@
       <c r="C35" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>32</v>
       </c>
@@ -1182,8 +1209,14 @@
       <c r="C36" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>33</v>
       </c>
@@ -1193,8 +1226,14 @@
       <c r="C37" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>34</v>
       </c>
@@ -1205,7 +1244,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>35</v>
       </c>
@@ -1216,7 +1255,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>36</v>
       </c>
@@ -1227,7 +1266,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>37</v>
       </c>
@@ -1238,7 +1277,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>38</v>
       </c>
@@ -1249,7 +1288,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>39</v>
       </c>
@@ -1260,7 +1299,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>40</v>
       </c>
@@ -1271,7 +1310,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>41</v>
       </c>
@@ -1282,7 +1321,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>42</v>
       </c>
@@ -1291,6 +1330,12 @@
       </c>
       <c r="C46" t="s">
         <v>97</v>
+      </c>
+      <c r="D46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E46" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
menambahkan new category company
</commit_message>
<xml_diff>
--- a/Business Category List.xlsx
+++ b/Business Category List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\html-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88570EF6-193B-4646-993B-799AFAA51E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1076D344-C85B-459D-9365-903C3703EC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3030" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
   <si>
     <t>Event Organizer</t>
   </si>
@@ -343,9 +343,6 @@
   </si>
   <si>
     <t>commersial</t>
-  </si>
-  <si>
-    <t>Prosess</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1195,7 @@
         <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add real estate, agency, job, consulting, startup, ecommerce, startup
</commit_message>
<xml_diff>
--- a/Business Category List.xlsx
+++ b/Business Category List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\html-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1076D344-C85B-459D-9365-903C3703EC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30DDC69-DFB0-40FD-8EAA-69C05EB13B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="106">
   <si>
     <t>Event Organizer</t>
   </si>
@@ -697,28 +697,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="105" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="2" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -738,7 +738,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -758,7 +758,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -778,7 +778,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -798,7 +798,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -818,7 +818,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -838,7 +838,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -858,7 +858,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -875,7 +875,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -892,7 +892,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>
@@ -909,7 +909,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10</v>
       </c>
@@ -926,7 +926,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
@@ -943,7 +943,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>12</v>
       </c>
@@ -960,7 +960,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
@@ -977,7 +977,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
@@ -994,7 +994,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>23</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>24</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>27</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>28</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>29</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>30</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>31</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>32</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>33</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>34</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>35</v>
       </c>
@@ -1344,8 +1344,14 @@
       <c r="C39" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>36</v>
       </c>
@@ -1355,8 +1361,14 @@
       <c r="C40" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>37</v>
       </c>
@@ -1366,8 +1378,14 @@
       <c r="C41" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>38</v>
       </c>
@@ -1377,8 +1395,14 @@
       <c r="C42" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>98</v>
+      </c>
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>39</v>
       </c>
@@ -1388,8 +1412,14 @@
       <c r="C43" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>40</v>
       </c>
@@ -1399,8 +1429,14 @@
       <c r="C44" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>41</v>
       </c>
@@ -1410,8 +1446,14 @@
       <c r="C45" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>42</v>
       </c>

</xml_diff>